<commit_message>
Added tests for a spot being full
</commit_message>
<xml_diff>
--- a/models/mock-data/Spots.xlsx
+++ b/models/mock-data/Spots.xlsx
@@ -1069,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="D224" sqref="D224"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1306,7 +1306,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1416,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1622,10 +1622,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1724,7 +1724,7 @@
         <v>0</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -2128,10 +2128,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C96">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -2428,7 +2428,7 @@
         <v>0</v>
       </c>
       <c r="C123">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
@@ -2436,10 +2436,10 @@
         <v>123</v>
       </c>
       <c r="B124" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C124">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
@@ -2667,10 +2667,10 @@
         <v>144</v>
       </c>
       <c r="B145" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C145">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>